<commit_message>
redef study area, split by seasons
</commit_message>
<xml_diff>
--- a/3.results/comptage_par_espece2.xlsx
+++ b/3.results/comptage_par_espece2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\schroll\Documents\stage_M2\3.results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63FDAD40-712A-4E1F-84E2-F72D43E9D0B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E51B2640-250F-4986-B3BF-9F03523ABC60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
   <si>
     <t>nom_fr</t>
   </si>
@@ -161,18 +161,6 @@
   </si>
   <si>
     <t>sterne moyenne ind</t>
-  </si>
-  <si>
-    <t>mars</t>
-  </si>
-  <si>
-    <t>juillet</t>
-  </si>
-  <si>
-    <t>avril</t>
-  </si>
-  <si>
-    <t>oct</t>
   </si>
 </sst>
 </file>
@@ -605,10 +593,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H42"/>
+  <dimension ref="A1:F42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A17"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -621,7 +609,7 @@
     <col min="6" max="6" width="12.140625" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -641,7 +629,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>6</v>
       </c>
@@ -661,7 +649,7 @@
         <v>4331</v>
       </c>
     </row>
-    <row r="3" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>7</v>
       </c>
@@ -680,14 +668,8 @@
       <c r="F3" s="4">
         <v>1435</v>
       </c>
-      <c r="G3" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="H3" s="5" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>8</v>
       </c>
@@ -703,7 +685,7 @@
         <v>934</v>
       </c>
     </row>
-    <row r="5" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>9</v>
       </c>
@@ -723,7 +705,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="6" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>10</v>
       </c>
@@ -743,7 +725,7 @@
         <v>552</v>
       </c>
     </row>
-    <row r="7" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>11</v>
       </c>
@@ -762,14 +744,8 @@
       <c r="F7" s="4">
         <v>210</v>
       </c>
-      <c r="G7" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="H7" s="5" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
         <v>12</v>
       </c>
@@ -785,7 +761,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>13</v>
       </c>
@@ -801,7 +777,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="10" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>14</v>
       </c>
@@ -821,7 +797,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="11" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
         <v>15</v>
       </c>
@@ -837,7 +813,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="12" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
         <v>16</v>
       </c>
@@ -853,7 +829,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="13" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
         <v>17</v>
       </c>
@@ -865,7 +841,7 @@
       <c r="E13" s="8"/>
       <c r="F13" s="8"/>
     </row>
-    <row r="14" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
         <v>18</v>
       </c>
@@ -879,7 +855,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
         <v>19</v>
       </c>
@@ -899,7 +875,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="16" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="10" t="s">
         <v>20</v>
       </c>

</xml_diff>

<commit_message>
add functions pt 2
</commit_message>
<xml_diff>
--- a/3.results/comptage_par_espece2.xlsx
+++ b/3.results/comptage_par_espece2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\schroll\Documents\stage_M2\3.results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32D4128A-9620-44A4-83A4-D22E3364FD0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A66C7760-8610-4123-B3C7-74161FE787D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -184,7 +184,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -215,6 +215,24 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -228,7 +246,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -258,6 +276,16 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -598,8 +626,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -749,7 +777,7 @@
       </c>
     </row>
     <row r="8" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="8" t="s">
+      <c r="A8" s="13" t="s">
         <v>12</v>
       </c>
       <c r="B8" s="8">
@@ -781,7 +809,7 @@
       </c>
     </row>
     <row r="10" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="6" t="s">
+      <c r="A10" s="16" t="s">
         <v>14</v>
       </c>
       <c r="B10" s="6">
@@ -817,7 +845,7 @@
       </c>
     </row>
     <row r="12" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="8" t="s">
+      <c r="A12" s="13" t="s">
         <v>16</v>
       </c>
       <c r="B12" s="8">
@@ -833,7 +861,7 @@
       </c>
     </row>
     <row r="13" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="8" t="s">
+      <c r="A13" s="15" t="s">
         <v>17</v>
       </c>
       <c r="B13" s="8">
@@ -845,7 +873,7 @@
       <c r="F13" s="8"/>
     </row>
     <row r="14" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="8" t="s">
+      <c r="A14" s="15" t="s">
         <v>18</v>
       </c>
       <c r="B14" s="8">
@@ -1089,23 +1117,31 @@
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="3" t="s">
+    <row r="33" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="E33" s="3">
+      <c r="B33" s="13"/>
+      <c r="C33" s="13"/>
+      <c r="D33" s="13"/>
+      <c r="E33" s="13">
         <v>4</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="3" t="s">
+      <c r="F33" s="13"/>
+    </row>
+    <row r="34" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="D34" s="3">
+      <c r="B34" s="13"/>
+      <c r="C34" s="13"/>
+      <c r="D34" s="13">
         <v>37</v>
       </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E34" s="13"/>
+      <c r="F34" s="13"/>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="10" t="s">
         <v>39</v>
       </c>
@@ -1113,7 +1149,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
         <v>40</v>
       </c>
@@ -1121,7 +1157,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
         <v>41</v>
       </c>
@@ -1129,8 +1165,8 @@
         <v>4</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" s="3" t="s">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" s="16" t="s">
         <v>42</v>
       </c>
       <c r="C38" s="3">
@@ -1140,15 +1176,19 @@
         <v>82</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" s="3" t="s">
+    <row r="39" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="D39" s="3">
+      <c r="B39" s="13"/>
+      <c r="C39" s="13"/>
+      <c r="D39" s="13">
         <v>52</v>
       </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E39" s="13"/>
+      <c r="F39" s="13"/>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
         <v>44</v>
       </c>
@@ -1156,7 +1196,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
         <v>45</v>
       </c>
@@ -1164,7 +1204,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
         <v>46</v>
       </c>

</xml_diff>